<commit_message>
:sparkles: added data and video analysis with descriptive statistics
</commit_message>
<xml_diff>
--- a/data/seminar6/Video_filtered_channels.xlsx
+++ b/data/seminar6/Video_filtered_channels.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM238"/>
+  <dimension ref="A1:AN238"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,6 +629,11 @@
           <t>liveStreamingDetails.scheduledStartTime</t>
         </is>
       </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>categoryName</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -790,6 +795,11 @@
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -991,6 +1001,11 @@
       <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1164,6 +1179,11 @@
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1353,6 +1373,11 @@
       <c r="AK5" t="inlineStr"/>
       <c r="AL5" t="inlineStr"/>
       <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1570,6 +1595,11 @@
       <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="inlineStr"/>
       <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1803,6 +1833,11 @@
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1980,6 +2015,11 @@
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="inlineStr"/>
       <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2197,6 +2237,11 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2406,6 +2451,11 @@
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="inlineStr"/>
       <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2615,6 +2665,11 @@
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr"/>
       <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2842,6 +2897,11 @@
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3011,6 +3071,11 @@
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3240,6 +3305,11 @@
       <c r="AK14" t="inlineStr"/>
       <c r="AL14" t="inlineStr"/>
       <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3449,6 +3519,11 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3626,6 +3701,11 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3803,6 +3883,11 @@
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="inlineStr"/>
       <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3986,6 +4071,11 @@
       <c r="AK18" t="inlineStr"/>
       <c r="AL18" t="inlineStr"/>
       <c r="AM18" t="inlineStr"/>
+      <c r="AN18" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -4201,6 +4291,11 @@
       <c r="AK19" t="inlineStr"/>
       <c r="AL19" t="inlineStr"/>
       <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -4408,6 +4503,11 @@
       <c r="AK20" t="inlineStr"/>
       <c r="AL20" t="inlineStr"/>
       <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -4637,6 +4737,11 @@
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -4850,6 +4955,11 @@
       <c r="AK22" t="inlineStr"/>
       <c r="AL22" t="inlineStr"/>
       <c r="AM22" t="inlineStr"/>
+      <c r="AN22" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -5079,6 +5189,11 @@
       <c r="AK23" t="inlineStr"/>
       <c r="AL23" t="inlineStr"/>
       <c r="AM23" t="inlineStr"/>
+      <c r="AN23" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -5278,6 +5393,11 @@
       <c r="AK24" t="inlineStr"/>
       <c r="AL24" t="inlineStr"/>
       <c r="AM24" t="inlineStr"/>
+      <c r="AN24" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -5457,6 +5577,11 @@
       <c r="AK25" t="inlineStr"/>
       <c r="AL25" t="inlineStr"/>
       <c r="AM25" t="inlineStr"/>
+      <c r="AN25" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -5674,6 +5799,11 @@
       <c r="AK26" t="inlineStr"/>
       <c r="AL26" t="inlineStr"/>
       <c r="AM26" t="inlineStr"/>
+      <c r="AN26" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -5853,6 +5983,11 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr">
+        <is>
+          <t>Entertainment</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -6072,6 +6207,11 @@
       <c r="AK28" t="inlineStr"/>
       <c r="AL28" t="inlineStr"/>
       <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -6211,6 +6351,11 @@
       <c r="AK29" t="inlineStr"/>
       <c r="AL29" t="inlineStr"/>
       <c r="AM29" t="inlineStr"/>
+      <c r="AN29" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -6424,6 +6569,11 @@
       <c r="AK30" t="inlineStr"/>
       <c r="AL30" t="inlineStr"/>
       <c r="AM30" t="inlineStr"/>
+      <c r="AN30" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -6579,6 +6729,11 @@
       <c r="AK31" t="inlineStr"/>
       <c r="AL31" t="inlineStr"/>
       <c r="AM31" t="inlineStr"/>
+      <c r="AN31" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -6798,6 +6953,11 @@
       <c r="AK32" t="inlineStr"/>
       <c r="AL32" t="inlineStr"/>
       <c r="AM32" t="inlineStr"/>
+      <c r="AN32" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -7003,6 +7163,11 @@
       <c r="AK33" t="inlineStr"/>
       <c r="AL33" t="inlineStr"/>
       <c r="AM33" t="inlineStr"/>
+      <c r="AN33" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -7168,6 +7333,11 @@
       <c r="AK34" t="inlineStr"/>
       <c r="AL34" t="inlineStr"/>
       <c r="AM34" t="inlineStr"/>
+      <c r="AN34" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -7405,6 +7575,11 @@
       <c r="AK35" t="inlineStr"/>
       <c r="AL35" t="inlineStr"/>
       <c r="AM35" t="inlineStr"/>
+      <c r="AN35" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -7548,6 +7723,11 @@
       <c r="AK36" t="inlineStr"/>
       <c r="AL36" t="inlineStr"/>
       <c r="AM36" t="inlineStr"/>
+      <c r="AN36" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -7811,6 +7991,11 @@
       <c r="AK37" t="inlineStr"/>
       <c r="AL37" t="inlineStr"/>
       <c r="AM37" t="inlineStr"/>
+      <c r="AN37" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -7966,6 +8151,11 @@
       <c r="AK38" t="inlineStr"/>
       <c r="AL38" t="inlineStr"/>
       <c r="AM38" t="inlineStr"/>
+      <c r="AN38" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -8143,6 +8333,11 @@
       <c r="AK39" t="inlineStr"/>
       <c r="AL39" t="inlineStr"/>
       <c r="AM39" t="inlineStr"/>
+      <c r="AN39" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -8304,6 +8499,11 @@
       <c r="AK40" t="inlineStr"/>
       <c r="AL40" t="inlineStr"/>
       <c r="AM40" t="inlineStr"/>
+      <c r="AN40" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -8477,6 +8677,11 @@
       <c r="AK41" t="inlineStr"/>
       <c r="AL41" t="inlineStr"/>
       <c r="AM41" t="inlineStr"/>
+      <c r="AN41" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -8622,6 +8827,11 @@
       <c r="AK42" t="inlineStr"/>
       <c r="AL42" t="inlineStr"/>
       <c r="AM42" t="inlineStr"/>
+      <c r="AN42" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -8801,6 +9011,11 @@
       <c r="AK43" t="inlineStr"/>
       <c r="AL43" t="inlineStr"/>
       <c r="AM43" t="inlineStr"/>
+      <c r="AN43" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -8940,6 +9155,11 @@
       <c r="AK44" t="inlineStr"/>
       <c r="AL44" t="inlineStr"/>
       <c r="AM44" t="inlineStr"/>
+      <c r="AN44" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -9157,6 +9377,11 @@
       <c r="AK45" t="inlineStr"/>
       <c r="AL45" t="inlineStr"/>
       <c r="AM45" t="inlineStr"/>
+      <c r="AN45" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -9320,6 +9545,11 @@
       <c r="AK46" t="inlineStr"/>
       <c r="AL46" t="inlineStr"/>
       <c r="AM46" t="inlineStr"/>
+      <c r="AN46" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -9511,6 +9741,11 @@
       <c r="AK47" t="inlineStr"/>
       <c r="AL47" t="inlineStr"/>
       <c r="AM47" t="inlineStr"/>
+      <c r="AN47" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -9716,6 +9951,11 @@
       <c r="AK48" t="inlineStr"/>
       <c r="AL48" t="inlineStr"/>
       <c r="AM48" t="inlineStr"/>
+      <c r="AN48" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -9923,6 +10163,11 @@
       <c r="AK49" t="inlineStr"/>
       <c r="AL49" t="inlineStr"/>
       <c r="AM49" t="inlineStr"/>
+      <c r="AN49" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -10116,6 +10361,11 @@
       <c r="AK50" t="inlineStr"/>
       <c r="AL50" t="inlineStr"/>
       <c r="AM50" t="inlineStr"/>
+      <c r="AN50" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -10269,6 +10519,11 @@
       <c r="AK51" t="inlineStr"/>
       <c r="AL51" t="inlineStr"/>
       <c r="AM51" t="inlineStr"/>
+      <c r="AN51" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -10428,6 +10683,11 @@
       <c r="AK52" t="inlineStr"/>
       <c r="AL52" t="inlineStr"/>
       <c r="AM52" t="inlineStr"/>
+      <c r="AN52" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -10649,6 +10909,11 @@
       <c r="AK53" t="inlineStr"/>
       <c r="AL53" t="inlineStr"/>
       <c r="AM53" t="inlineStr"/>
+      <c r="AN53" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -10888,6 +11153,11 @@
       <c r="AK54" t="inlineStr"/>
       <c r="AL54" t="inlineStr"/>
       <c r="AM54" t="inlineStr"/>
+      <c r="AN54" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -11133,6 +11403,11 @@
       <c r="AK55" t="inlineStr"/>
       <c r="AL55" t="inlineStr"/>
       <c r="AM55" t="inlineStr"/>
+      <c r="AN55" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -11340,6 +11615,11 @@
       <c r="AK56" t="inlineStr"/>
       <c r="AL56" t="inlineStr"/>
       <c r="AM56" t="inlineStr"/>
+      <c r="AN56" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -11503,6 +11783,11 @@
       <c r="AK57" t="inlineStr"/>
       <c r="AL57" t="inlineStr"/>
       <c r="AM57" t="inlineStr"/>
+      <c r="AN57" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -11686,6 +11971,11 @@
       <c r="AK58" t="inlineStr"/>
       <c r="AL58" t="inlineStr"/>
       <c r="AM58" t="inlineStr"/>
+      <c r="AN58" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -11933,6 +12223,11 @@
       <c r="AK59" t="inlineStr"/>
       <c r="AL59" t="inlineStr"/>
       <c r="AM59" t="inlineStr"/>
+      <c r="AN59" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -12150,6 +12445,11 @@
       <c r="AK60" t="inlineStr"/>
       <c r="AL60" t="inlineStr"/>
       <c r="AM60" t="inlineStr"/>
+      <c r="AN60" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -12359,6 +12659,11 @@
       <c r="AK61" t="inlineStr"/>
       <c r="AL61" t="inlineStr"/>
       <c r="AM61" t="inlineStr"/>
+      <c r="AN61" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -12514,6 +12819,11 @@
       <c r="AK62" t="inlineStr"/>
       <c r="AL62" t="inlineStr"/>
       <c r="AM62" t="inlineStr"/>
+      <c r="AN62" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -12725,6 +13035,11 @@
       <c r="AK63" t="inlineStr"/>
       <c r="AL63" t="inlineStr"/>
       <c r="AM63" t="inlineStr"/>
+      <c r="AN63" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -12914,6 +13229,11 @@
       <c r="AK64" t="inlineStr"/>
       <c r="AL64" t="inlineStr"/>
       <c r="AM64" t="inlineStr"/>
+      <c r="AN64" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -13087,6 +13407,11 @@
       <c r="AK65" t="inlineStr"/>
       <c r="AL65" t="inlineStr"/>
       <c r="AM65" t="inlineStr"/>
+      <c r="AN65" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -13260,6 +13585,11 @@
       <c r="AK66" t="inlineStr"/>
       <c r="AL66" t="inlineStr"/>
       <c r="AM66" t="inlineStr"/>
+      <c r="AN66" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -13463,6 +13793,11 @@
           <t>2020-03-14T12:00:00Z</t>
         </is>
       </c>
+      <c r="AN67" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -13628,6 +13963,11 @@
       <c r="AK68" t="inlineStr"/>
       <c r="AL68" t="inlineStr"/>
       <c r="AM68" t="inlineStr"/>
+      <c r="AN68" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -13817,6 +14157,11 @@
       <c r="AK69" t="inlineStr"/>
       <c r="AL69" t="inlineStr"/>
       <c r="AM69" t="inlineStr"/>
+      <c r="AN69" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -13992,6 +14337,11 @@
       <c r="AK70" t="inlineStr"/>
       <c r="AL70" t="inlineStr"/>
       <c r="AM70" t="inlineStr"/>
+      <c r="AN70" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -14149,6 +14499,11 @@
       <c r="AK71" t="inlineStr"/>
       <c r="AL71" t="inlineStr"/>
       <c r="AM71" t="inlineStr"/>
+      <c r="AN71" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -14384,6 +14739,11 @@
       <c r="AK72" t="inlineStr"/>
       <c r="AL72" t="inlineStr"/>
       <c r="AM72" t="inlineStr"/>
+      <c r="AN72" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -14595,6 +14955,11 @@
           <t>2021-11-12T14:45:00Z</t>
         </is>
       </c>
+      <c r="AN73" t="inlineStr">
+        <is>
+          <t>Travel &amp; Events</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -14760,6 +15125,11 @@
       <c r="AK74" t="inlineStr"/>
       <c r="AL74" t="inlineStr"/>
       <c r="AM74" t="inlineStr"/>
+      <c r="AN74" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -14947,6 +15317,11 @@
       <c r="AK75" t="inlineStr"/>
       <c r="AL75" t="inlineStr"/>
       <c r="AM75" t="inlineStr"/>
+      <c r="AN75" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -15162,6 +15537,11 @@
       <c r="AK76" t="inlineStr"/>
       <c r="AL76" t="inlineStr"/>
       <c r="AM76" t="inlineStr"/>
+      <c r="AN76" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -15399,6 +15779,11 @@
       <c r="AK77" t="inlineStr"/>
       <c r="AL77" t="inlineStr"/>
       <c r="AM77" t="inlineStr"/>
+      <c r="AN77" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -15586,6 +15971,11 @@
       <c r="AK78" t="inlineStr"/>
       <c r="AL78" t="inlineStr"/>
       <c r="AM78" t="inlineStr"/>
+      <c r="AN78" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -15773,6 +16163,11 @@
       <c r="AK79" t="inlineStr"/>
       <c r="AL79" t="inlineStr"/>
       <c r="AM79" t="inlineStr"/>
+      <c r="AN79" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -15944,6 +16339,11 @@
       <c r="AK80" t="inlineStr"/>
       <c r="AL80" t="inlineStr"/>
       <c r="AM80" t="inlineStr"/>
+      <c r="AN80" t="inlineStr">
+        <is>
+          <t>Film &amp; Animation</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -16123,6 +16523,11 @@
       <c r="AK81" t="inlineStr"/>
       <c r="AL81" t="inlineStr"/>
       <c r="AM81" t="inlineStr"/>
+      <c r="AN81" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -16276,6 +16681,11 @@
       <c r="AK82" t="inlineStr"/>
       <c r="AL82" t="inlineStr"/>
       <c r="AM82" t="inlineStr"/>
+      <c r="AN82" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -16459,6 +16869,11 @@
       <c r="AK83" t="inlineStr"/>
       <c r="AL83" t="inlineStr"/>
       <c r="AM83" t="inlineStr"/>
+      <c r="AN83" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -16656,6 +17071,11 @@
       <c r="AK84" t="inlineStr"/>
       <c r="AL84" t="inlineStr"/>
       <c r="AM84" t="inlineStr"/>
+      <c r="AN84" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -16857,6 +17277,11 @@
       <c r="AK85" t="inlineStr"/>
       <c r="AL85" t="inlineStr"/>
       <c r="AM85" t="inlineStr"/>
+      <c r="AN85" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -17044,6 +17469,11 @@
       <c r="AK86" t="inlineStr"/>
       <c r="AL86" t="inlineStr"/>
       <c r="AM86" t="inlineStr"/>
+      <c r="AN86" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -17213,6 +17643,11 @@
       <c r="AK87" t="inlineStr"/>
       <c r="AL87" t="inlineStr"/>
       <c r="AM87" t="inlineStr"/>
+      <c r="AN87" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -17432,6 +17867,11 @@
       <c r="AK88" t="inlineStr"/>
       <c r="AL88" t="inlineStr"/>
       <c r="AM88" t="inlineStr"/>
+      <c r="AN88" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -17685,6 +18125,11 @@
       <c r="AK89" t="inlineStr"/>
       <c r="AL89" t="inlineStr"/>
       <c r="AM89" t="inlineStr"/>
+      <c r="AN89" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -17914,6 +18359,11 @@
       <c r="AK90" t="inlineStr"/>
       <c r="AL90" t="inlineStr"/>
       <c r="AM90" t="inlineStr"/>
+      <c r="AN90" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -18133,6 +18583,11 @@
       <c r="AK91" t="inlineStr"/>
       <c r="AL91" t="inlineStr"/>
       <c r="AM91" t="inlineStr"/>
+      <c r="AN91" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -18298,6 +18753,11 @@
       <c r="AK92" t="inlineStr"/>
       <c r="AL92" t="inlineStr"/>
       <c r="AM92" t="inlineStr"/>
+      <c r="AN92" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -18491,6 +18951,11 @@
       <c r="AK93" t="inlineStr"/>
       <c r="AL93" t="inlineStr"/>
       <c r="AM93" t="inlineStr"/>
+      <c r="AN93" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -18658,6 +19123,11 @@
       <c r="AK94" t="inlineStr"/>
       <c r="AL94" t="inlineStr"/>
       <c r="AM94" t="inlineStr"/>
+      <c r="AN94" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -18899,6 +19369,11 @@
       <c r="AK95" t="inlineStr"/>
       <c r="AL95" t="inlineStr"/>
       <c r="AM95" t="inlineStr"/>
+      <c r="AN95" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -19084,6 +19559,11 @@
       <c r="AK96" t="inlineStr"/>
       <c r="AL96" t="inlineStr"/>
       <c r="AM96" t="inlineStr"/>
+      <c r="AN96" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -19313,6 +19793,11 @@
       <c r="AK97" t="inlineStr"/>
       <c r="AL97" t="inlineStr"/>
       <c r="AM97" t="inlineStr"/>
+      <c r="AN97" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -19496,6 +19981,11 @@
       <c r="AK98" t="inlineStr"/>
       <c r="AL98" t="inlineStr"/>
       <c r="AM98" t="inlineStr"/>
+      <c r="AN98" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -19651,6 +20141,11 @@
       <c r="AK99" t="inlineStr"/>
       <c r="AL99" t="inlineStr"/>
       <c r="AM99" t="inlineStr"/>
+      <c r="AN99" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -19900,6 +20395,11 @@
       <c r="AK100" t="inlineStr"/>
       <c r="AL100" t="inlineStr"/>
       <c r="AM100" t="inlineStr"/>
+      <c r="AN100" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -20053,6 +20553,11 @@
       <c r="AK101" t="inlineStr"/>
       <c r="AL101" t="inlineStr"/>
       <c r="AM101" t="inlineStr"/>
+      <c r="AN101" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -20250,6 +20755,11 @@
       <c r="AK102" t="inlineStr"/>
       <c r="AL102" t="inlineStr"/>
       <c r="AM102" t="inlineStr"/>
+      <c r="AN102" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -20407,6 +20917,11 @@
       <c r="AK103" t="inlineStr"/>
       <c r="AL103" t="inlineStr"/>
       <c r="AM103" t="inlineStr"/>
+      <c r="AN103" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -20602,6 +21117,11 @@
       <c r="AK104" t="inlineStr"/>
       <c r="AL104" t="inlineStr"/>
       <c r="AM104" t="inlineStr"/>
+      <c r="AN104" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -20799,6 +21319,11 @@
       <c r="AK105" t="inlineStr"/>
       <c r="AL105" t="inlineStr"/>
       <c r="AM105" t="inlineStr"/>
+      <c r="AN105" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -20952,6 +21477,11 @@
       <c r="AK106" t="inlineStr"/>
       <c r="AL106" t="inlineStr"/>
       <c r="AM106" t="inlineStr"/>
+      <c r="AN106" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -21131,6 +21661,11 @@
       <c r="AK107" t="inlineStr"/>
       <c r="AL107" t="inlineStr"/>
       <c r="AM107" t="inlineStr"/>
+      <c r="AN107" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -21316,6 +21851,11 @@
       <c r="AK108" t="inlineStr"/>
       <c r="AL108" t="inlineStr"/>
       <c r="AM108" t="inlineStr"/>
+      <c r="AN108" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -21477,6 +22017,11 @@
       <c r="AK109" t="inlineStr"/>
       <c r="AL109" t="inlineStr"/>
       <c r="AM109" t="inlineStr"/>
+      <c r="AN109" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -21676,6 +22221,11 @@
       <c r="AK110" t="inlineStr"/>
       <c r="AL110" t="inlineStr"/>
       <c r="AM110" t="inlineStr"/>
+      <c r="AN110" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -21961,6 +22511,11 @@
       <c r="AK111" t="inlineStr"/>
       <c r="AL111" t="inlineStr"/>
       <c r="AM111" t="inlineStr"/>
+      <c r="AN111" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -22202,6 +22757,11 @@
       <c r="AK112" t="inlineStr"/>
       <c r="AL112" t="inlineStr"/>
       <c r="AM112" t="inlineStr"/>
+      <c r="AN112" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -22369,6 +22929,11 @@
       <c r="AK113" t="inlineStr"/>
       <c r="AL113" t="inlineStr"/>
       <c r="AM113" t="inlineStr"/>
+      <c r="AN113" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -22586,6 +23151,11 @@
       <c r="AK114" t="inlineStr"/>
       <c r="AL114" t="inlineStr"/>
       <c r="AM114" t="inlineStr"/>
+      <c r="AN114" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -22783,6 +23353,11 @@
       <c r="AK115" t="inlineStr"/>
       <c r="AL115" t="inlineStr"/>
       <c r="AM115" t="inlineStr"/>
+      <c r="AN115" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -23012,6 +23587,11 @@
       <c r="AK116" t="inlineStr"/>
       <c r="AL116" t="inlineStr"/>
       <c r="AM116" t="inlineStr"/>
+      <c r="AN116" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -23189,6 +23769,11 @@
       <c r="AK117" t="inlineStr"/>
       <c r="AL117" t="inlineStr"/>
       <c r="AM117" t="inlineStr"/>
+      <c r="AN117" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -23372,6 +23957,11 @@
       <c r="AK118" t="inlineStr"/>
       <c r="AL118" t="inlineStr"/>
       <c r="AM118" t="inlineStr"/>
+      <c r="AN118" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -23667,6 +24257,11 @@
       <c r="AK119" t="inlineStr"/>
       <c r="AL119" t="inlineStr"/>
       <c r="AM119" t="inlineStr"/>
+      <c r="AN119" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -23904,6 +24499,11 @@
       <c r="AK120" t="inlineStr"/>
       <c r="AL120" t="inlineStr"/>
       <c r="AM120" t="inlineStr"/>
+      <c r="AN120" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -24159,6 +24759,11 @@
       <c r="AK121" t="inlineStr"/>
       <c r="AL121" t="inlineStr"/>
       <c r="AM121" t="inlineStr"/>
+      <c r="AN121" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -24298,6 +24903,11 @@
       <c r="AK122" t="inlineStr"/>
       <c r="AL122" t="inlineStr"/>
       <c r="AM122" t="inlineStr"/>
+      <c r="AN122" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -24485,6 +25095,11 @@
       <c r="AK123" t="inlineStr"/>
       <c r="AL123" t="inlineStr"/>
       <c r="AM123" t="inlineStr"/>
+      <c r="AN123" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -24744,6 +25359,11 @@
       <c r="AK124" t="inlineStr"/>
       <c r="AL124" t="inlineStr"/>
       <c r="AM124" t="inlineStr"/>
+      <c r="AN124" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -24957,6 +25577,11 @@
       <c r="AK125" t="inlineStr"/>
       <c r="AL125" t="inlineStr"/>
       <c r="AM125" t="inlineStr"/>
+      <c r="AN125" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -25172,6 +25797,11 @@
       <c r="AK126" t="inlineStr"/>
       <c r="AL126" t="inlineStr"/>
       <c r="AM126" t="inlineStr"/>
+      <c r="AN126" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -25383,6 +26013,11 @@
       <c r="AK127" t="inlineStr"/>
       <c r="AL127" t="inlineStr"/>
       <c r="AM127" t="inlineStr"/>
+      <c r="AN127" t="inlineStr">
+        <is>
+          <t>Travel &amp; Events</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -25582,6 +26217,11 @@
       <c r="AK128" t="inlineStr"/>
       <c r="AL128" t="inlineStr"/>
       <c r="AM128" t="inlineStr"/>
+      <c r="AN128" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -25817,6 +26457,11 @@
       <c r="AK129" t="inlineStr"/>
       <c r="AL129" t="inlineStr"/>
       <c r="AM129" t="inlineStr"/>
+      <c r="AN129" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -26112,6 +26757,11 @@
       <c r="AK130" t="inlineStr"/>
       <c r="AL130" t="inlineStr"/>
       <c r="AM130" t="inlineStr"/>
+      <c r="AN130" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -26275,6 +26925,11 @@
       <c r="AK131" t="inlineStr"/>
       <c r="AL131" t="inlineStr"/>
       <c r="AM131" t="inlineStr"/>
+      <c r="AN131" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -26446,6 +27101,11 @@
       <c r="AM132" t="inlineStr">
         <is>
           <t>2020-06-25T13:15:00Z</t>
+        </is>
+      </c>
+      <c r="AN132" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
         </is>
       </c>
     </row>
@@ -26671,6 +27331,11 @@
       <c r="AK133" t="inlineStr"/>
       <c r="AL133" t="inlineStr"/>
       <c r="AM133" t="inlineStr"/>
+      <c r="AN133" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -26918,6 +27583,11 @@
       <c r="AK134" t="inlineStr"/>
       <c r="AL134" t="inlineStr"/>
       <c r="AM134" t="inlineStr"/>
+      <c r="AN134" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -27091,6 +27761,11 @@
       <c r="AK135" t="inlineStr"/>
       <c r="AL135" t="inlineStr"/>
       <c r="AM135" t="inlineStr"/>
+      <c r="AN135" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -27258,6 +27933,11 @@
       <c r="AK136" t="inlineStr"/>
       <c r="AL136" t="inlineStr"/>
       <c r="AM136" t="inlineStr"/>
+      <c r="AN136" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -27445,6 +28125,11 @@
       <c r="AK137" t="inlineStr"/>
       <c r="AL137" t="inlineStr"/>
       <c r="AM137" t="inlineStr"/>
+      <c r="AN137" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -27664,6 +28349,11 @@
       <c r="AK138" t="inlineStr"/>
       <c r="AL138" t="inlineStr"/>
       <c r="AM138" t="inlineStr"/>
+      <c r="AN138" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -27887,6 +28577,11 @@
       <c r="AK139" t="inlineStr"/>
       <c r="AL139" t="inlineStr"/>
       <c r="AM139" t="inlineStr"/>
+      <c r="AN139" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -28088,6 +28783,11 @@
       <c r="AK140" t="inlineStr"/>
       <c r="AL140" t="inlineStr"/>
       <c r="AM140" t="inlineStr"/>
+      <c r="AN140" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -28237,6 +28937,11 @@
       <c r="AK141" t="inlineStr"/>
       <c r="AL141" t="inlineStr"/>
       <c r="AM141" t="inlineStr"/>
+      <c r="AN141" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -28422,6 +29127,11 @@
       <c r="AK142" t="inlineStr"/>
       <c r="AL142" t="inlineStr"/>
       <c r="AM142" t="inlineStr"/>
+      <c r="AN142" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -28655,6 +29365,11 @@
       <c r="AK143" t="inlineStr"/>
       <c r="AL143" t="inlineStr"/>
       <c r="AM143" t="inlineStr"/>
+      <c r="AN143" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -28878,6 +29593,11 @@
       <c r="AK144" t="inlineStr"/>
       <c r="AL144" t="inlineStr"/>
       <c r="AM144" t="inlineStr"/>
+      <c r="AN144" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -29085,6 +29805,11 @@
       <c r="AK145" t="inlineStr"/>
       <c r="AL145" t="inlineStr"/>
       <c r="AM145" t="inlineStr"/>
+      <c r="AN145" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -29308,6 +30033,11 @@
       <c r="AK146" t="inlineStr"/>
       <c r="AL146" t="inlineStr"/>
       <c r="AM146" t="inlineStr"/>
+      <c r="AN146" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -29535,6 +30265,11 @@
       <c r="AK147" t="inlineStr"/>
       <c r="AL147" t="inlineStr"/>
       <c r="AM147" t="inlineStr"/>
+      <c r="AN147" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -29718,6 +30453,11 @@
       <c r="AK148" t="inlineStr"/>
       <c r="AL148" t="inlineStr"/>
       <c r="AM148" t="inlineStr"/>
+      <c r="AN148" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -29965,6 +30705,11 @@
       <c r="AK149" t="inlineStr"/>
       <c r="AL149" t="inlineStr"/>
       <c r="AM149" t="inlineStr"/>
+      <c r="AN149" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -30204,6 +30949,11 @@
       <c r="AK150" t="inlineStr"/>
       <c r="AL150" t="inlineStr"/>
       <c r="AM150" t="inlineStr"/>
+      <c r="AN150" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -30357,6 +31107,11 @@
       <c r="AK151" t="inlineStr"/>
       <c r="AL151" t="inlineStr"/>
       <c r="AM151" t="inlineStr"/>
+      <c r="AN151" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -30516,6 +31271,11 @@
       <c r="AK152" t="inlineStr"/>
       <c r="AL152" t="inlineStr"/>
       <c r="AM152" t="inlineStr"/>
+      <c r="AN152" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -30691,6 +31451,11 @@
       <c r="AK153" t="inlineStr"/>
       <c r="AL153" t="inlineStr"/>
       <c r="AM153" t="inlineStr"/>
+      <c r="AN153" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -30858,6 +31623,11 @@
       <c r="AK154" t="inlineStr"/>
       <c r="AL154" t="inlineStr"/>
       <c r="AM154" t="inlineStr"/>
+      <c r="AN154" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -31075,6 +31845,11 @@
       <c r="AK155" t="inlineStr"/>
       <c r="AL155" t="inlineStr"/>
       <c r="AM155" t="inlineStr"/>
+      <c r="AN155" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -31246,6 +32021,11 @@
       <c r="AK156" t="inlineStr"/>
       <c r="AL156" t="inlineStr"/>
       <c r="AM156" t="inlineStr"/>
+      <c r="AN156" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -31449,6 +32229,11 @@
       <c r="AK157" t="inlineStr"/>
       <c r="AL157" t="inlineStr"/>
       <c r="AM157" t="inlineStr"/>
+      <c r="AN157" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -31684,6 +32469,11 @@
       <c r="AK158" t="inlineStr"/>
       <c r="AL158" t="inlineStr"/>
       <c r="AM158" t="inlineStr"/>
+      <c r="AN158" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -31841,6 +32631,11 @@
       <c r="AK159" t="inlineStr"/>
       <c r="AL159" t="inlineStr"/>
       <c r="AM159" t="inlineStr"/>
+      <c r="AN159" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -32070,6 +32865,11 @@
       <c r="AK160" t="inlineStr"/>
       <c r="AL160" t="inlineStr"/>
       <c r="AM160" t="inlineStr"/>
+      <c r="AN160" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -32263,6 +33063,11 @@
       <c r="AK161" t="inlineStr"/>
       <c r="AL161" t="inlineStr"/>
       <c r="AM161" t="inlineStr"/>
+      <c r="AN161" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -32456,6 +33261,11 @@
       <c r="AK162" t="inlineStr"/>
       <c r="AL162" t="inlineStr"/>
       <c r="AM162" t="inlineStr"/>
+      <c r="AN162" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -32637,6 +33447,11 @@
       <c r="AK163" t="inlineStr"/>
       <c r="AL163" t="inlineStr"/>
       <c r="AM163" t="inlineStr"/>
+      <c r="AN163" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -32872,6 +33687,11 @@
       <c r="AK164" t="inlineStr"/>
       <c r="AL164" t="inlineStr"/>
       <c r="AM164" t="inlineStr"/>
+      <c r="AN164" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -33031,6 +33851,11 @@
       <c r="AK165" t="inlineStr"/>
       <c r="AL165" t="inlineStr"/>
       <c r="AM165" t="inlineStr"/>
+      <c r="AN165" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -33254,6 +34079,11 @@
       <c r="AK166" t="inlineStr"/>
       <c r="AL166" t="inlineStr"/>
       <c r="AM166" t="inlineStr"/>
+      <c r="AN166" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -33463,6 +34293,11 @@
       <c r="AK167" t="inlineStr"/>
       <c r="AL167" t="inlineStr"/>
       <c r="AM167" t="inlineStr"/>
+      <c r="AN167" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -33636,6 +34471,11 @@
       <c r="AK168" t="inlineStr"/>
       <c r="AL168" t="inlineStr"/>
       <c r="AM168" t="inlineStr"/>
+      <c r="AN168" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -33869,6 +34709,11 @@
       <c r="AK169" t="inlineStr"/>
       <c r="AL169" t="inlineStr"/>
       <c r="AM169" t="inlineStr"/>
+      <c r="AN169" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -34042,6 +34887,11 @@
       <c r="AK170" t="inlineStr"/>
       <c r="AL170" t="inlineStr"/>
       <c r="AM170" t="inlineStr"/>
+      <c r="AN170" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -34181,6 +35031,11 @@
       <c r="AK171" t="inlineStr"/>
       <c r="AL171" t="inlineStr"/>
       <c r="AM171" t="inlineStr"/>
+      <c r="AN171" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -34384,6 +35239,11 @@
       <c r="AK172" t="inlineStr"/>
       <c r="AL172" t="inlineStr"/>
       <c r="AM172" t="inlineStr"/>
+      <c r="AN172" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -34599,6 +35459,11 @@
       <c r="AK173" t="inlineStr"/>
       <c r="AL173" t="inlineStr"/>
       <c r="AM173" t="inlineStr"/>
+      <c r="AN173" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -34804,6 +35669,11 @@
       <c r="AK174" t="inlineStr"/>
       <c r="AL174" t="inlineStr"/>
       <c r="AM174" t="inlineStr"/>
+      <c r="AN174" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -35013,6 +35883,11 @@
       <c r="AK175" t="inlineStr"/>
       <c r="AL175" t="inlineStr"/>
       <c r="AM175" t="inlineStr"/>
+      <c r="AN175" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -35260,6 +36135,11 @@
       <c r="AK176" t="inlineStr"/>
       <c r="AL176" t="inlineStr"/>
       <c r="AM176" t="inlineStr"/>
+      <c r="AN176" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -35487,6 +36367,11 @@
       <c r="AK177" t="inlineStr"/>
       <c r="AL177" t="inlineStr"/>
       <c r="AM177" t="inlineStr"/>
+      <c r="AN177" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -35678,6 +36563,11 @@
       <c r="AK178" t="inlineStr"/>
       <c r="AL178" t="inlineStr"/>
       <c r="AM178" t="inlineStr"/>
+      <c r="AN178" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -35897,6 +36787,11 @@
       <c r="AK179" t="inlineStr"/>
       <c r="AL179" t="inlineStr"/>
       <c r="AM179" t="inlineStr"/>
+      <c r="AN179" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -36122,6 +37017,11 @@
       <c r="AK180" t="inlineStr"/>
       <c r="AL180" t="inlineStr"/>
       <c r="AM180" t="inlineStr"/>
+      <c r="AN180" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -36339,6 +37239,11 @@
       <c r="AK181" t="inlineStr"/>
       <c r="AL181" t="inlineStr"/>
       <c r="AM181" t="inlineStr"/>
+      <c r="AN181" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -36546,6 +37451,11 @@
       <c r="AK182" t="inlineStr"/>
       <c r="AL182" t="inlineStr"/>
       <c r="AM182" t="inlineStr"/>
+      <c r="AN182" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -36793,6 +37703,11 @@
       <c r="AK183" t="inlineStr"/>
       <c r="AL183" t="inlineStr"/>
       <c r="AM183" t="inlineStr"/>
+      <c r="AN183" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -37006,6 +37921,11 @@
       <c r="AK184" t="inlineStr"/>
       <c r="AL184" t="inlineStr"/>
       <c r="AM184" t="inlineStr"/>
+      <c r="AN184" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -37217,6 +38137,11 @@
       <c r="AK185" t="inlineStr"/>
       <c r="AL185" t="inlineStr"/>
       <c r="AM185" t="inlineStr"/>
+      <c r="AN185" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -37392,6 +38317,11 @@
       <c r="AK186" t="inlineStr"/>
       <c r="AL186" t="inlineStr"/>
       <c r="AM186" t="inlineStr"/>
+      <c r="AN186" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -37581,6 +38511,11 @@
       <c r="AK187" t="inlineStr"/>
       <c r="AL187" t="inlineStr"/>
       <c r="AM187" t="inlineStr"/>
+      <c r="AN187" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -37796,6 +38731,11 @@
       <c r="AK188" t="inlineStr"/>
       <c r="AL188" t="inlineStr"/>
       <c r="AM188" t="inlineStr"/>
+      <c r="AN188" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -38021,6 +38961,11 @@
       <c r="AK189" t="inlineStr"/>
       <c r="AL189" t="inlineStr"/>
       <c r="AM189" t="inlineStr"/>
+      <c r="AN189" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -38220,6 +39165,11 @@
       <c r="AK190" t="inlineStr"/>
       <c r="AL190" t="inlineStr"/>
       <c r="AM190" t="inlineStr"/>
+      <c r="AN190" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -38447,6 +39397,11 @@
       <c r="AK191" t="inlineStr"/>
       <c r="AL191" t="inlineStr"/>
       <c r="AM191" t="inlineStr"/>
+      <c r="AN191" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -38608,6 +39563,11 @@
       <c r="AK192" t="inlineStr"/>
       <c r="AL192" t="inlineStr"/>
       <c r="AM192" t="inlineStr"/>
+      <c r="AN192" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -38775,6 +39735,11 @@
       <c r="AK193" t="inlineStr"/>
       <c r="AL193" t="inlineStr"/>
       <c r="AM193" t="inlineStr"/>
+      <c r="AN193" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -39022,6 +39987,11 @@
       <c r="AK194" t="inlineStr"/>
       <c r="AL194" t="inlineStr"/>
       <c r="AM194" t="inlineStr"/>
+      <c r="AN194" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -39211,6 +40181,11 @@
       <c r="AK195" t="inlineStr"/>
       <c r="AL195" t="inlineStr"/>
       <c r="AM195" t="inlineStr"/>
+      <c r="AN195" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -39412,6 +40387,11 @@
       <c r="AK196" t="inlineStr"/>
       <c r="AL196" t="inlineStr"/>
       <c r="AM196" t="inlineStr"/>
+      <c r="AN196" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -39579,6 +40559,11 @@
       <c r="AK197" t="inlineStr"/>
       <c r="AL197" t="inlineStr"/>
       <c r="AM197" t="inlineStr"/>
+      <c r="AN197" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -39788,6 +40773,11 @@
       <c r="AK198" t="inlineStr"/>
       <c r="AL198" t="inlineStr"/>
       <c r="AM198" t="inlineStr"/>
+      <c r="AN198" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -39989,6 +40979,11 @@
       <c r="AK199" t="inlineStr"/>
       <c r="AL199" t="inlineStr"/>
       <c r="AM199" t="inlineStr"/>
+      <c r="AN199" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -40180,6 +41175,11 @@
       <c r="AK200" t="inlineStr"/>
       <c r="AL200" t="inlineStr"/>
       <c r="AM200" t="inlineStr"/>
+      <c r="AN200" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -40365,6 +41365,11 @@
       <c r="AK201" t="inlineStr"/>
       <c r="AL201" t="inlineStr"/>
       <c r="AM201" t="inlineStr"/>
+      <c r="AN201" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -40606,6 +41611,11 @@
           <t>2023-03-03T04:00:00Z</t>
         </is>
       </c>
+      <c r="AN202" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -40783,6 +41793,11 @@
       <c r="AK203" t="inlineStr"/>
       <c r="AL203" t="inlineStr"/>
       <c r="AM203" t="inlineStr"/>
+      <c r="AN203" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -40954,6 +41969,11 @@
       <c r="AK204" t="inlineStr"/>
       <c r="AL204" t="inlineStr"/>
       <c r="AM204" t="inlineStr"/>
+      <c r="AN204" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -41093,6 +42113,11 @@
       <c r="AK205" t="inlineStr"/>
       <c r="AL205" t="inlineStr"/>
       <c r="AM205" t="inlineStr"/>
+      <c r="AN205" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -41256,6 +42281,11 @@
       <c r="AK206" t="inlineStr"/>
       <c r="AL206" t="inlineStr"/>
       <c r="AM206" t="inlineStr"/>
+      <c r="AN206" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -41411,6 +42441,11 @@
       <c r="AK207" t="inlineStr"/>
       <c r="AL207" t="inlineStr"/>
       <c r="AM207" t="inlineStr"/>
+      <c r="AN207" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -41574,6 +42609,11 @@
       <c r="AK208" t="inlineStr"/>
       <c r="AL208" t="inlineStr"/>
       <c r="AM208" t="inlineStr"/>
+      <c r="AN208" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -41791,6 +42831,11 @@
       <c r="AK209" t="inlineStr"/>
       <c r="AL209" t="inlineStr"/>
       <c r="AM209" t="inlineStr"/>
+      <c r="AN209" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -41954,6 +42999,11 @@
       <c r="AK210" t="inlineStr"/>
       <c r="AL210" t="inlineStr"/>
       <c r="AM210" t="inlineStr"/>
+      <c r="AN210" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -42179,6 +43229,11 @@
       <c r="AK211" t="inlineStr"/>
       <c r="AL211" t="inlineStr"/>
       <c r="AM211" t="inlineStr"/>
+      <c r="AN211" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -42400,6 +43455,11 @@
       <c r="AK212" t="inlineStr"/>
       <c r="AL212" t="inlineStr"/>
       <c r="AM212" t="inlineStr"/>
+      <c r="AN212" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -42563,6 +43623,11 @@
       <c r="AK213" t="inlineStr"/>
       <c r="AL213" t="inlineStr"/>
       <c r="AM213" t="inlineStr"/>
+      <c r="AN213" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -42718,6 +43783,11 @@
       <c r="AK214" t="inlineStr"/>
       <c r="AL214" t="inlineStr"/>
       <c r="AM214" t="inlineStr"/>
+      <c r="AN214" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -42937,6 +44007,11 @@
       <c r="AK215" t="inlineStr"/>
       <c r="AL215" t="inlineStr"/>
       <c r="AM215" t="inlineStr"/>
+      <c r="AN215" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -43158,6 +44233,11 @@
       <c r="AK216" t="inlineStr"/>
       <c r="AL216" t="inlineStr"/>
       <c r="AM216" t="inlineStr"/>
+      <c r="AN216" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -43325,6 +44405,11 @@
       <c r="AK217" t="inlineStr"/>
       <c r="AL217" t="inlineStr"/>
       <c r="AM217" t="inlineStr"/>
+      <c r="AN217" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -43478,6 +44563,11 @@
       <c r="AK218" t="inlineStr"/>
       <c r="AL218" t="inlineStr"/>
       <c r="AM218" t="inlineStr"/>
+      <c r="AN218" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -43699,6 +44789,11 @@
       <c r="AK219" t="inlineStr"/>
       <c r="AL219" t="inlineStr"/>
       <c r="AM219" t="inlineStr"/>
+      <c r="AN219" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -43860,6 +44955,11 @@
       <c r="AK220" t="inlineStr"/>
       <c r="AL220" t="inlineStr"/>
       <c r="AM220" t="inlineStr"/>
+      <c r="AN220" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -44051,6 +45151,11 @@
       <c r="AK221" t="inlineStr"/>
       <c r="AL221" t="inlineStr"/>
       <c r="AM221" t="inlineStr"/>
+      <c r="AN221" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -44204,6 +45309,11 @@
       <c r="AK222" t="inlineStr"/>
       <c r="AL222" t="inlineStr"/>
       <c r="AM222" t="inlineStr"/>
+      <c r="AN222" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -44379,6 +45489,11 @@
       <c r="AK223" t="inlineStr"/>
       <c r="AL223" t="inlineStr"/>
       <c r="AM223" t="inlineStr"/>
+      <c r="AN223" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -44574,6 +45689,11 @@
       <c r="AK224" t="inlineStr"/>
       <c r="AL224" t="inlineStr"/>
       <c r="AM224" t="inlineStr"/>
+      <c r="AN224" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -44799,6 +45919,11 @@
       <c r="AK225" t="inlineStr"/>
       <c r="AL225" t="inlineStr"/>
       <c r="AM225" t="inlineStr"/>
+      <c r="AN225" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -44964,6 +46089,11 @@
       <c r="AK226" t="inlineStr"/>
       <c r="AL226" t="inlineStr"/>
       <c r="AM226" t="inlineStr"/>
+      <c r="AN226" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -45121,6 +46251,11 @@
       <c r="AK227" t="inlineStr"/>
       <c r="AL227" t="inlineStr"/>
       <c r="AM227" t="inlineStr"/>
+      <c r="AN227" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -45316,6 +46451,11 @@
       <c r="AK228" t="inlineStr"/>
       <c r="AL228" t="inlineStr"/>
       <c r="AM228" t="inlineStr"/>
+      <c r="AN228" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -45479,6 +46619,11 @@
       <c r="AK229" t="inlineStr"/>
       <c r="AL229" t="inlineStr"/>
       <c r="AM229" t="inlineStr"/>
+      <c r="AN229" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -45652,6 +46797,11 @@
       <c r="AK230" t="inlineStr"/>
       <c r="AL230" t="inlineStr"/>
       <c r="AM230" t="inlineStr"/>
+      <c r="AN230" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -45813,6 +46963,11 @@
       <c r="AK231" t="inlineStr"/>
       <c r="AL231" t="inlineStr"/>
       <c r="AM231" t="inlineStr"/>
+      <c r="AN231" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -46048,6 +47203,11 @@
       <c r="AK232" t="inlineStr"/>
       <c r="AL232" t="inlineStr"/>
       <c r="AM232" t="inlineStr"/>
+      <c r="AN232" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -46253,6 +47413,11 @@
       <c r="AK233" t="inlineStr"/>
       <c r="AL233" t="inlineStr"/>
       <c r="AM233" t="inlineStr"/>
+      <c r="AN233" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -46392,6 +47557,11 @@
       <c r="AK234" t="inlineStr"/>
       <c r="AL234" t="inlineStr"/>
       <c r="AM234" t="inlineStr"/>
+      <c r="AN234" t="inlineStr">
+        <is>
+          <t>People &amp; Blogs</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -46577,6 +47747,11 @@
       <c r="AK235" t="inlineStr"/>
       <c r="AL235" t="inlineStr"/>
       <c r="AM235" t="inlineStr"/>
+      <c r="AN235" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -46732,6 +47907,11 @@
       <c r="AK236" t="inlineStr"/>
       <c r="AL236" t="inlineStr"/>
       <c r="AM236" t="inlineStr"/>
+      <c r="AN236" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -46887,6 +48067,11 @@
       <c r="AK237" t="inlineStr"/>
       <c r="AL237" t="inlineStr"/>
       <c r="AM237" t="inlineStr"/>
+      <c r="AN237" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -47060,6 +48245,11 @@
       <c r="AK238" t="inlineStr"/>
       <c r="AL238" t="inlineStr"/>
       <c r="AM238" t="inlineStr"/>
+      <c r="AN238" t="inlineStr">
+        <is>
+          <t>Howto &amp; Style</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>